<commit_message>
Disctricts list excel updated with 1 new disctrict
Ko'kdala district of Kashkadarya region was added. 
Sources:
https://senat.uz/uz/lists/view/4132
https://www.gazeta.uz/oz/2022/03/17/kokdala/
</commit_message>
<xml_diff>
--- a/excel/districts-uzb.xlsx
+++ b/excel/districts-uzb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AK\Desktop\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ak/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EBAF10-1777-4D53-8406-F0ED5444FDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25C895A-5EAC-144E-AAC2-A9CA4636A37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19095" yWindow="6120" windowWidth="15375" windowHeight="7875" tabRatio="451" xr2:uid="{5883D59D-79A6-644C-90C1-2DD3C01115E6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" tabRatio="451" xr2:uid="{5883D59D-79A6-644C-90C1-2DD3C01115E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tumalar- districts" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="638">
   <si>
     <t>id</t>
   </si>
@@ -1930,6 +1930,15 @@
   </si>
   <si>
     <t>Region_name</t>
+  </si>
+  <si>
+    <t>Ko'kdala tumani</t>
+  </si>
+  <si>
+    <t>Кукдалинский район</t>
+  </si>
+  <si>
+    <t>Кўкдала тумани</t>
   </si>
 </sst>
 </file>
@@ -2401,25 +2410,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2AD5AB4-134A-4A49-823C-CD04E6C40220}">
   <dimension ref="A1:I732"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="109" workbookViewId="0">
+      <selection activeCell="B208" sqref="B208"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.875" customWidth="1"/>
-    <col min="2" max="2" width="37.25" customWidth="1"/>
-    <col min="3" max="3" width="30.625" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="37.1640625" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="10.5" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="9.875" customWidth="1"/>
-    <col min="8" max="8" width="25.375" customWidth="1"/>
-    <col min="9" max="9" width="35.125" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" customWidth="1"/>
+    <col min="9" max="9" width="35.1640625" customWidth="1"/>
     <col min="10" max="10" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2439,7 +2448,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2461,7 +2470,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2483,7 +2492,7 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2505,7 +2514,7 @@
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2527,7 +2536,7 @@
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2549,7 +2558,7 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2571,7 +2580,7 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2593,7 +2602,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2615,7 +2624,7 @@
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2637,7 +2646,7 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2659,7 +2668,7 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2681,7 +2690,7 @@
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2703,7 +2712,7 @@
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2725,7 +2734,7 @@
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2747,7 +2756,7 @@
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2767,7 +2776,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2787,7 +2796,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2807,7 +2816,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2827,7 +2836,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2847,7 +2856,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2867,7 +2876,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2887,7 +2896,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2907,7 +2916,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2927,7 +2936,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2947,7 +2956,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2967,7 +2976,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2987,7 +2996,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3007,7 +3016,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3027,7 +3036,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3047,7 +3056,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3067,7 +3076,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3087,7 +3096,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3107,7 +3116,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3127,7 +3136,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3147,7 +3156,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3167,7 +3176,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3187,7 +3196,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3207,7 +3216,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3227,7 +3236,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3247,7 +3256,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3267,7 +3276,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3287,7 +3296,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3307,7 +3316,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3327,7 +3336,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3347,7 +3356,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3367,7 +3376,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3387,7 +3396,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3407,7 +3416,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3427,7 +3436,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3447,7 +3456,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3467,7 +3476,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3487,7 +3496,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3507,7 +3516,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3527,7 +3536,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3547,7 +3556,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3567,7 +3576,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3587,7 +3596,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3607,7 +3616,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3627,7 +3636,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3647,7 +3656,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3667,7 +3676,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3687,7 +3696,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3707,7 +3716,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3727,7 +3736,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3747,7 +3756,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3767,7 +3776,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3787,7 +3796,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3807,7 +3816,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3827,7 +3836,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3847,7 +3856,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3867,7 +3876,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3887,7 +3896,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3907,7 +3916,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3927,7 +3936,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3947,7 +3956,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3967,7 +3976,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3987,7 +3996,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4007,7 +4016,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4027,7 +4036,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4047,7 +4056,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4067,7 +4076,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4087,7 +4096,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4107,7 +4116,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4127,7 +4136,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4147,7 +4156,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4167,7 +4176,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4187,7 +4196,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4207,7 +4216,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4227,7 +4236,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4247,7 +4256,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4267,7 +4276,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4287,7 +4296,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4307,7 +4316,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4327,7 +4336,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4347,7 +4356,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4367,7 +4376,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4387,7 +4396,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4407,7 +4416,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4427,7 +4436,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4447,7 +4456,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4467,7 +4476,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4487,7 +4496,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4507,7 +4516,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4527,7 +4536,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4547,7 +4556,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4567,7 +4576,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4587,7 +4596,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4607,7 +4616,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4627,7 +4636,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4647,7 +4656,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4667,7 +4676,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4687,7 +4696,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4707,7 +4716,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4727,7 +4736,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4747,7 +4756,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4767,7 +4776,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4787,7 +4796,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4807,7 +4816,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -4827,7 +4836,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -4847,7 +4856,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -4867,7 +4876,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4887,7 +4896,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4907,7 +4916,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4927,7 +4936,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4947,7 +4956,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4967,7 +4976,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4987,7 +4996,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5007,7 +5016,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -5027,7 +5036,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5047,7 +5056,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5067,7 +5076,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -5087,7 +5096,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5107,7 +5116,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5127,7 +5136,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5147,7 +5156,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5167,7 +5176,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5187,7 +5196,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5207,7 +5216,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5227,7 +5236,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5247,7 +5256,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5267,7 +5276,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5287,7 +5296,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5307,7 +5316,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -5327,7 +5336,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -5347,7 +5356,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -5367,7 +5376,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -5387,7 +5396,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -5407,7 +5416,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -5427,7 +5436,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -5447,7 +5456,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -5467,7 +5476,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -5487,7 +5496,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
@@ -5507,7 +5516,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
@@ -5527,7 +5536,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
@@ -5547,7 +5556,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
@@ -5567,7 +5576,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
@@ -5587,7 +5596,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>157</v>
       </c>
@@ -5607,7 +5616,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>158</v>
       </c>
@@ -5627,7 +5636,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>159</v>
       </c>
@@ -5647,7 +5656,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>160</v>
       </c>
@@ -5667,7 +5676,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>161</v>
       </c>
@@ -5687,7 +5696,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>162</v>
       </c>
@@ -5707,7 +5716,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>163</v>
       </c>
@@ -5727,7 +5736,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>164</v>
       </c>
@@ -5747,7 +5756,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>165</v>
       </c>
@@ -5767,7 +5776,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>166</v>
       </c>
@@ -5787,7 +5796,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>167</v>
       </c>
@@ -5807,7 +5816,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>168</v>
       </c>
@@ -5827,7 +5836,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>169</v>
       </c>
@@ -5847,7 +5856,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>170</v>
       </c>
@@ -5867,7 +5876,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>171</v>
       </c>
@@ -5887,7 +5896,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>172</v>
       </c>
@@ -5907,7 +5916,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>173</v>
       </c>
@@ -5927,7 +5936,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>174</v>
       </c>
@@ -5947,7 +5956,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>175</v>
       </c>
@@ -5967,7 +5976,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>176</v>
       </c>
@@ -5987,7 +5996,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>177</v>
       </c>
@@ -6007,7 +6016,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>178</v>
       </c>
@@ -6027,7 +6036,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>179</v>
       </c>
@@ -6047,7 +6056,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>180</v>
       </c>
@@ -6067,7 +6076,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>181</v>
       </c>
@@ -6087,7 +6096,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>182</v>
       </c>
@@ -6107,7 +6116,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>183</v>
       </c>
@@ -6127,7 +6136,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>184</v>
       </c>
@@ -6147,7 +6156,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>185</v>
       </c>
@@ -6167,7 +6176,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>186</v>
       </c>
@@ -6187,7 +6196,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>187</v>
       </c>
@@ -6207,7 +6216,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>188</v>
       </c>
@@ -6227,7 +6236,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>189</v>
       </c>
@@ -6247,7 +6256,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>190</v>
       </c>
@@ -6267,7 +6276,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>191</v>
       </c>
@@ -6287,7 +6296,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>192</v>
       </c>
@@ -6307,7 +6316,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>193</v>
       </c>
@@ -6327,7 +6336,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>194</v>
       </c>
@@ -6347,7 +6356,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>195</v>
       </c>
@@ -6367,7 +6376,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>196</v>
       </c>
@@ -6387,7 +6396,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>197</v>
       </c>
@@ -6407,7 +6416,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>198</v>
       </c>
@@ -6427,7 +6436,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>199</v>
       </c>
@@ -6447,7 +6456,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>200</v>
       </c>
@@ -6467,7 +6476,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>201</v>
       </c>
@@ -6487,7 +6496,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>202</v>
       </c>
@@ -6507,7 +6516,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>203</v>
       </c>
@@ -6527,7 +6536,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>204</v>
       </c>
@@ -6547,7 +6556,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>205</v>
       </c>
@@ -6567,2440 +6576,2460 @@
         <v>632</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207" t="s">
+        <v>635</v>
+      </c>
+      <c r="C207" t="s">
+        <v>637</v>
+      </c>
+      <c r="D207" t="s">
+        <v>636</v>
+      </c>
+      <c r="E207" s="7">
+        <v>9</v>
+      </c>
+      <c r="F207" s="13" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" s="4"/>
     </row>
-    <row r="246" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A246" s="1"/>
       <c r="C246" s="3"/>
       <c r="E246" s="1"/>
     </row>
-    <row r="247" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A247" s="1"/>
       <c r="C247" s="3"/>
       <c r="E247" s="1"/>
     </row>
-    <row r="248" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A248" s="1"/>
       <c r="C248" s="3"/>
       <c r="E248" s="1"/>
     </row>
-    <row r="249" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A249" s="1"/>
       <c r="C249" s="3"/>
       <c r="E249" s="1"/>
     </row>
-    <row r="250" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A250" s="1"/>
       <c r="C250" s="3"/>
       <c r="E250" s="1"/>
     </row>
-    <row r="251" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A251" s="1"/>
       <c r="C251" s="3"/>
       <c r="E251" s="1"/>
     </row>
-    <row r="252" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A252" s="1"/>
       <c r="C252" s="3"/>
       <c r="E252" s="1"/>
     </row>
-    <row r="253" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A253" s="1"/>
       <c r="C253" s="2"/>
       <c r="E253" s="1"/>
     </row>
-    <row r="254" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A254" s="1"/>
       <c r="C254" s="2"/>
       <c r="E254" s="1"/>
     </row>
-    <row r="255" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A255" s="1"/>
       <c r="C255" s="2"/>
       <c r="E255" s="1"/>
     </row>
-    <row r="256" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A256" s="1"/>
       <c r="C256" s="3"/>
       <c r="E256" s="1"/>
     </row>
-    <row r="257" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A257" s="1"/>
       <c r="C257" s="3"/>
       <c r="E257" s="1"/>
     </row>
-    <row r="258" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A258" s="1"/>
       <c r="C258" s="3"/>
       <c r="E258" s="1"/>
     </row>
-    <row r="259" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A259" s="1"/>
       <c r="C259" s="3"/>
       <c r="E259" s="1"/>
     </row>
-    <row r="260" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A260" s="1"/>
       <c r="C260" s="3"/>
       <c r="E260" s="1"/>
     </row>
-    <row r="261" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A261" s="1"/>
       <c r="C261" s="3"/>
       <c r="E261" s="1"/>
     </row>
-    <row r="262" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A262" s="1"/>
       <c r="C262" s="2"/>
       <c r="E262" s="1"/>
     </row>
-    <row r="263" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A263" s="1"/>
       <c r="C263" s="2"/>
       <c r="E263" s="1"/>
     </row>
-    <row r="264" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A264" s="1"/>
       <c r="C264" s="2"/>
       <c r="E264" s="1"/>
     </row>
-    <row r="265" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A265" s="1"/>
       <c r="C265" s="2"/>
       <c r="E265" s="1"/>
     </row>
-    <row r="266" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A266" s="1"/>
       <c r="C266" s="2"/>
       <c r="E266" s="1"/>
     </row>
-    <row r="267" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A267" s="1"/>
       <c r="C267" s="2"/>
       <c r="E267" s="1"/>
     </row>
-    <row r="268" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A268" s="1"/>
       <c r="C268" s="2"/>
       <c r="E268" s="1"/>
     </row>
-    <row r="269" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A269" s="1"/>
       <c r="C269" s="2"/>
       <c r="E269" s="1"/>
     </row>
-    <row r="270" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A270" s="1"/>
       <c r="C270" s="2"/>
       <c r="E270" s="1"/>
     </row>
-    <row r="271" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A271" s="1"/>
       <c r="C271" s="2"/>
       <c r="E271" s="1"/>
     </row>
-    <row r="272" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A272" s="1"/>
       <c r="C272" s="2"/>
       <c r="E272" s="1"/>
     </row>
-    <row r="273" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A273" s="1"/>
       <c r="C273" s="2"/>
       <c r="E273" s="1"/>
     </row>
-    <row r="274" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A274" s="1"/>
       <c r="C274" s="3"/>
       <c r="E274" s="1"/>
     </row>
-    <row r="275" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A275" s="1"/>
       <c r="C275" s="3"/>
       <c r="E275" s="1"/>
     </row>
-    <row r="276" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A276" s="1"/>
       <c r="C276" s="3"/>
       <c r="E276" s="1"/>
     </row>
-    <row r="277" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A277" s="1"/>
       <c r="C277" s="2"/>
       <c r="E277" s="1"/>
     </row>
-    <row r="278" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A278" s="1"/>
       <c r="C278" s="2"/>
       <c r="E278" s="1"/>
     </row>
-    <row r="279" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A279" s="1"/>
       <c r="C279" s="2"/>
       <c r="E279" s="1"/>
     </row>
-    <row r="280" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A280" s="1"/>
       <c r="C280" s="2"/>
       <c r="E280" s="1"/>
     </row>
-    <row r="281" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A281" s="1"/>
       <c r="C281" s="2"/>
       <c r="E281" s="1"/>
     </row>
-    <row r="282" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A282" s="1"/>
       <c r="C282" s="2"/>
       <c r="E282" s="1"/>
     </row>
-    <row r="283" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A283" s="1"/>
       <c r="C283" s="2"/>
       <c r="E283" s="1"/>
     </row>
-    <row r="284" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A284" s="1"/>
       <c r="C284" s="2"/>
       <c r="E284" s="1"/>
     </row>
-    <row r="285" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A285" s="1"/>
       <c r="C285" s="2"/>
       <c r="E285" s="1"/>
     </row>
-    <row r="286" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A286" s="1"/>
       <c r="C286" s="2"/>
       <c r="E286" s="1"/>
     </row>
-    <row r="287" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A287" s="1"/>
       <c r="C287" s="2"/>
       <c r="E287" s="1"/>
     </row>
-    <row r="288" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A288" s="1"/>
       <c r="C288" s="2"/>
       <c r="E288" s="1"/>
     </row>
-    <row r="289" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A289" s="1"/>
       <c r="C289" s="2"/>
       <c r="E289" s="1"/>
     </row>
-    <row r="290" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A290" s="1"/>
       <c r="C290" s="2"/>
       <c r="E290" s="1"/>
     </row>
-    <row r="291" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A291" s="1"/>
       <c r="C291" s="2"/>
       <c r="E291" s="1"/>
     </row>
-    <row r="292" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A292" s="1"/>
       <c r="C292" s="2"/>
       <c r="E292" s="1"/>
     </row>
-    <row r="293" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A293" s="1"/>
       <c r="C293" s="2"/>
       <c r="E293" s="1"/>
     </row>
-    <row r="294" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A294" s="1"/>
       <c r="C294" s="2"/>
       <c r="E294" s="1"/>
     </row>
-    <row r="295" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A295" s="1"/>
       <c r="C295" s="2"/>
       <c r="E295" s="1"/>
     </row>
-    <row r="296" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A296" s="1"/>
       <c r="C296" s="2"/>
       <c r="E296" s="1"/>
     </row>
-    <row r="297" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A297" s="1"/>
       <c r="C297" s="2"/>
       <c r="E297" s="1"/>
     </row>
-    <row r="298" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A298" s="1"/>
       <c r="C298" s="2"/>
       <c r="E298" s="1"/>
     </row>
-    <row r="299" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A299" s="1"/>
       <c r="C299" s="2"/>
       <c r="E299" s="1"/>
     </row>
-    <row r="300" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A300" s="1"/>
       <c r="C300" s="2"/>
       <c r="E300" s="1"/>
     </row>
-    <row r="301" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A301" s="1"/>
       <c r="C301" s="2"/>
       <c r="E301" s="1"/>
     </row>
-    <row r="302" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A302" s="1"/>
       <c r="C302" s="2"/>
       <c r="E302" s="1"/>
     </row>
-    <row r="303" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A303" s="1"/>
       <c r="C303" s="2"/>
       <c r="E303" s="1"/>
     </row>
-    <row r="304" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A304" s="1"/>
       <c r="C304" s="2"/>
       <c r="E304" s="1"/>
     </row>
-    <row r="305" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A305" s="1"/>
       <c r="C305" s="2"/>
       <c r="E305" s="1"/>
     </row>
-    <row r="306" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A306" s="1"/>
       <c r="C306" s="2"/>
       <c r="E306" s="1"/>
     </row>
-    <row r="307" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A307" s="1"/>
       <c r="C307" s="2"/>
       <c r="E307" s="1"/>
     </row>
-    <row r="308" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A308" s="1"/>
       <c r="C308" s="2"/>
       <c r="E308" s="1"/>
     </row>
-    <row r="309" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A309" s="1"/>
       <c r="C309" s="2"/>
       <c r="E309" s="1"/>
     </row>
-    <row r="310" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A310" s="1"/>
       <c r="C310" s="2"/>
       <c r="E310" s="1"/>
     </row>
-    <row r="311" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A311" s="1"/>
       <c r="C311" s="2"/>
       <c r="E311" s="1"/>
     </row>
-    <row r="312" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A312" s="1"/>
       <c r="C312" s="2"/>
       <c r="E312" s="1"/>
     </row>
-    <row r="313" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A313" s="1"/>
       <c r="C313" s="3"/>
       <c r="E313" s="1"/>
     </row>
-    <row r="314" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A314" s="1"/>
       <c r="C314" s="3"/>
       <c r="E314" s="1"/>
     </row>
-    <row r="315" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A315" s="1"/>
       <c r="C315" s="3"/>
       <c r="E315" s="1"/>
     </row>
-    <row r="316" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A316" s="1"/>
       <c r="C316" s="2"/>
       <c r="E316" s="1"/>
     </row>
-    <row r="317" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A317" s="1"/>
       <c r="C317" s="2"/>
       <c r="E317" s="1"/>
     </row>
-    <row r="318" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A318" s="1"/>
       <c r="C318" s="2"/>
       <c r="E318" s="1"/>
     </row>
-    <row r="319" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A319" s="1"/>
       <c r="C319" s="2"/>
       <c r="E319" s="1"/>
     </row>
-    <row r="320" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A320" s="1"/>
       <c r="C320" s="2"/>
       <c r="E320" s="1"/>
     </row>
-    <row r="321" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A321" s="1"/>
       <c r="C321" s="2"/>
       <c r="E321" s="1"/>
     </row>
-    <row r="322" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A322" s="1"/>
       <c r="C322" s="2"/>
       <c r="E322" s="1"/>
     </row>
-    <row r="323" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A323" s="1"/>
       <c r="C323" s="2"/>
       <c r="E323" s="1"/>
     </row>
-    <row r="324" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A324" s="1"/>
       <c r="C324" s="2"/>
       <c r="E324" s="1"/>
     </row>
-    <row r="325" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A325" s="1"/>
       <c r="C325" s="3"/>
       <c r="E325" s="1"/>
     </row>
-    <row r="326" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A326" s="1"/>
       <c r="C326" s="3"/>
       <c r="E326" s="1"/>
     </row>
-    <row r="327" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A327" s="1"/>
       <c r="C327" s="3"/>
       <c r="E327" s="1"/>
     </row>
-    <row r="328" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A328" s="1"/>
       <c r="C328" s="2"/>
       <c r="E328" s="1"/>
     </row>
-    <row r="329" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A329" s="1"/>
       <c r="C329" s="2"/>
       <c r="E329" s="1"/>
     </row>
-    <row r="330" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A330" s="1"/>
       <c r="C330" s="2"/>
       <c r="E330" s="1"/>
     </row>
-    <row r="331" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A331" s="1"/>
       <c r="C331" s="3"/>
       <c r="E331" s="1"/>
     </row>
-    <row r="332" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A332" s="1"/>
       <c r="C332" s="3"/>
       <c r="E332" s="1"/>
     </row>
-    <row r="333" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A333" s="1"/>
       <c r="C333" s="3"/>
       <c r="E333" s="1"/>
     </row>
-    <row r="334" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A334" s="1"/>
       <c r="C334" s="2"/>
       <c r="E334" s="1"/>
     </row>
-    <row r="335" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A335" s="1"/>
       <c r="C335" s="2"/>
       <c r="E335" s="1"/>
     </row>
-    <row r="336" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A336" s="1"/>
       <c r="C336" s="2"/>
       <c r="E336" s="1"/>
     </row>
-    <row r="337" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A337" s="1"/>
       <c r="C337" s="2"/>
       <c r="E337" s="1"/>
     </row>
-    <row r="338" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A338" s="1"/>
       <c r="C338" s="2"/>
       <c r="E338" s="1"/>
     </row>
-    <row r="339" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A339" s="1"/>
       <c r="C339" s="2"/>
       <c r="E339" s="1"/>
     </row>
-    <row r="340" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A340" s="1"/>
       <c r="C340" s="2"/>
       <c r="E340" s="1"/>
     </row>
-    <row r="341" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A341" s="1"/>
       <c r="C341" s="2"/>
       <c r="E341" s="1"/>
     </row>
-    <row r="342" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A342" s="1"/>
       <c r="C342" s="2"/>
       <c r="E342" s="1"/>
     </row>
-    <row r="343" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A343" s="1"/>
       <c r="C343" s="2"/>
       <c r="E343" s="1"/>
     </row>
-    <row r="344" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A344" s="1"/>
       <c r="C344" s="2"/>
       <c r="E344" s="1"/>
     </row>
-    <row r="345" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A345" s="1"/>
       <c r="C345" s="2"/>
       <c r="E345" s="1"/>
     </row>
-    <row r="346" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A346" s="1"/>
       <c r="C346" s="2"/>
       <c r="E346" s="1"/>
     </row>
-    <row r="347" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A347" s="1"/>
       <c r="C347" s="2"/>
       <c r="E347" s="1"/>
     </row>
-    <row r="348" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A348" s="1"/>
       <c r="C348" s="2"/>
       <c r="E348" s="1"/>
     </row>
-    <row r="349" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A349" s="1"/>
       <c r="C349" s="3"/>
       <c r="E349" s="1"/>
     </row>
-    <row r="350" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A350" s="1"/>
       <c r="C350" s="3"/>
       <c r="E350" s="1"/>
     </row>
-    <row r="351" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A351" s="1"/>
       <c r="C351" s="3"/>
       <c r="E351" s="1"/>
     </row>
-    <row r="352" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A352" s="1"/>
       <c r="C352" s="2"/>
       <c r="E352" s="1"/>
     </row>
-    <row r="353" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A353" s="1"/>
       <c r="C353" s="2"/>
       <c r="E353" s="1"/>
     </row>
-    <row r="354" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A354" s="1"/>
       <c r="C354" s="2"/>
       <c r="E354" s="1"/>
     </row>
-    <row r="355" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A355" s="1"/>
       <c r="C355" s="3"/>
       <c r="E355" s="1"/>
     </row>
-    <row r="356" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A356" s="1"/>
       <c r="C356" s="3"/>
       <c r="E356" s="1"/>
     </row>
-    <row r="357" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A357" s="1"/>
       <c r="C357" s="3"/>
       <c r="E357" s="1"/>
     </row>
-    <row r="358" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A358" s="1"/>
       <c r="C358" s="2"/>
       <c r="E358" s="1"/>
     </row>
-    <row r="359" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A359" s="1"/>
       <c r="C359" s="2"/>
       <c r="E359" s="1"/>
     </row>
-    <row r="360" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A360" s="1"/>
       <c r="C360" s="2"/>
       <c r="E360" s="1"/>
     </row>
-    <row r="361" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A361" s="1"/>
       <c r="C361" s="2"/>
       <c r="E361" s="1"/>
     </row>
-    <row r="362" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A362" s="1"/>
       <c r="C362" s="2"/>
       <c r="E362" s="1"/>
     </row>
-    <row r="363" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A363" s="1"/>
       <c r="C363" s="2"/>
       <c r="E363" s="1"/>
     </row>
-    <row r="364" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A364" s="1"/>
       <c r="C364" s="2"/>
       <c r="E364" s="1"/>
     </row>
-    <row r="365" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A365" s="1"/>
       <c r="C365" s="2"/>
       <c r="E365" s="1"/>
     </row>
-    <row r="366" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A366" s="1"/>
       <c r="C366" s="2"/>
       <c r="E366" s="1"/>
     </row>
-    <row r="367" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A367" s="1"/>
       <c r="C367" s="2"/>
       <c r="E367" s="1"/>
     </row>
-    <row r="368" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A368" s="1"/>
       <c r="C368" s="2"/>
       <c r="E368" s="1"/>
     </row>
-    <row r="369" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A369" s="1"/>
       <c r="C369" s="2"/>
       <c r="E369" s="1"/>
     </row>
-    <row r="370" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A370" s="1"/>
       <c r="C370" s="2"/>
       <c r="E370" s="1"/>
     </row>
-    <row r="371" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A371" s="1"/>
       <c r="C371" s="2"/>
       <c r="E371" s="1"/>
     </row>
-    <row r="372" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A372" s="1"/>
       <c r="C372" s="2"/>
       <c r="E372" s="1"/>
     </row>
-    <row r="373" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A373" s="1"/>
       <c r="C373" s="3"/>
       <c r="E373" s="1"/>
     </row>
-    <row r="374" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A374" s="1"/>
       <c r="C374" s="3"/>
       <c r="E374" s="1"/>
     </row>
-    <row r="375" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A375" s="1"/>
       <c r="C375" s="3"/>
       <c r="E375" s="1"/>
     </row>
-    <row r="376" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A376" s="1"/>
       <c r="C376" s="2"/>
       <c r="E376" s="1"/>
     </row>
-    <row r="377" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A377" s="1"/>
       <c r="C377" s="2"/>
       <c r="E377" s="1"/>
     </row>
-    <row r="378" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A378" s="1"/>
       <c r="C378" s="2"/>
       <c r="E378" s="1"/>
     </row>
-    <row r="379" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A379" s="1"/>
       <c r="C379" s="3"/>
       <c r="E379" s="1"/>
     </row>
-    <row r="380" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A380" s="1"/>
       <c r="C380" s="3"/>
       <c r="E380" s="1"/>
     </row>
-    <row r="381" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A381" s="1"/>
       <c r="C381" s="3"/>
       <c r="E381" s="1"/>
     </row>
-    <row r="382" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A382" s="1"/>
       <c r="C382" s="3"/>
       <c r="E382" s="1"/>
     </row>
-    <row r="383" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A383" s="1"/>
       <c r="C383" s="3"/>
       <c r="E383" s="1"/>
     </row>
-    <row r="384" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A384" s="1"/>
       <c r="C384" s="3"/>
       <c r="E384" s="1"/>
     </row>
-    <row r="385" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A385" s="1"/>
       <c r="C385" s="2"/>
       <c r="E385" s="1"/>
     </row>
-    <row r="386" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A386" s="1"/>
       <c r="C386" s="2"/>
       <c r="E386" s="1"/>
     </row>
-    <row r="387" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A387" s="1"/>
       <c r="C387" s="2"/>
       <c r="E387" s="1"/>
     </row>
-    <row r="388" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A388" s="1"/>
       <c r="C388" s="2"/>
       <c r="E388" s="1"/>
     </row>
-    <row r="389" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A389" s="1"/>
       <c r="C389" s="2"/>
       <c r="E389" s="1"/>
     </row>
-    <row r="390" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A390" s="1"/>
       <c r="C390" s="2"/>
       <c r="E390" s="1"/>
     </row>
-    <row r="391" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A391" s="1"/>
       <c r="C391" s="2"/>
       <c r="E391" s="1"/>
     </row>
-    <row r="392" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A392" s="1"/>
       <c r="C392" s="2"/>
       <c r="E392" s="1"/>
     </row>
-    <row r="393" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A393" s="1"/>
       <c r="C393" s="2"/>
       <c r="E393" s="1"/>
     </row>
-    <row r="394" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A394" s="1"/>
       <c r="C394" s="2"/>
       <c r="E394" s="1"/>
     </row>
-    <row r="395" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A395" s="1"/>
       <c r="C395" s="2"/>
       <c r="E395" s="1"/>
     </row>
-    <row r="396" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A396" s="1"/>
       <c r="C396" s="2"/>
       <c r="E396" s="1"/>
     </row>
-    <row r="397" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A397" s="1"/>
       <c r="C397" s="2"/>
       <c r="E397" s="1"/>
     </row>
-    <row r="398" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A398" s="1"/>
       <c r="C398" s="2"/>
       <c r="E398" s="1"/>
     </row>
-    <row r="399" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A399" s="1"/>
       <c r="C399" s="2"/>
       <c r="E399" s="1"/>
     </row>
-    <row r="400" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A400" s="1"/>
       <c r="C400" s="2"/>
       <c r="E400" s="1"/>
     </row>
-    <row r="401" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A401" s="1"/>
       <c r="C401" s="2"/>
       <c r="E401" s="1"/>
     </row>
-    <row r="402" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A402" s="1"/>
       <c r="C402" s="2"/>
       <c r="E402" s="1"/>
     </row>
-    <row r="403" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A403" s="1"/>
       <c r="C403" s="2"/>
       <c r="E403" s="1"/>
     </row>
-    <row r="404" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A404" s="1"/>
       <c r="C404" s="2"/>
       <c r="E404" s="1"/>
     </row>
-    <row r="405" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A405" s="1"/>
       <c r="C405" s="2"/>
       <c r="E405" s="1"/>
     </row>
-    <row r="406" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A406" s="1"/>
       <c r="C406" s="2"/>
       <c r="E406" s="1"/>
     </row>
-    <row r="407" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A407" s="1"/>
       <c r="C407" s="2"/>
       <c r="E407" s="1"/>
     </row>
-    <row r="408" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A408" s="1"/>
       <c r="C408" s="2"/>
       <c r="E408" s="1"/>
     </row>
-    <row r="409" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A409" s="1"/>
       <c r="C409" s="2"/>
       <c r="E409" s="1"/>
     </row>
-    <row r="410" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A410" s="1"/>
       <c r="C410" s="2"/>
       <c r="E410" s="1"/>
     </row>
-    <row r="411" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A411" s="1"/>
       <c r="C411" s="2"/>
       <c r="E411" s="1"/>
     </row>
-    <row r="412" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A412" s="1"/>
       <c r="C412" s="2"/>
       <c r="E412" s="1"/>
     </row>
-    <row r="413" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A413" s="1"/>
       <c r="C413" s="2"/>
       <c r="E413" s="1"/>
     </row>
-    <row r="414" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A414" s="1"/>
       <c r="C414" s="2"/>
       <c r="E414" s="1"/>
     </row>
-    <row r="415" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A415" s="1"/>
       <c r="C415" s="2"/>
       <c r="E415" s="1"/>
     </row>
-    <row r="416" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A416" s="1"/>
       <c r="C416" s="2"/>
       <c r="E416" s="1"/>
     </row>
-    <row r="417" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A417" s="1"/>
       <c r="C417" s="2"/>
       <c r="E417" s="1"/>
     </row>
-    <row r="418" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A418" s="1"/>
       <c r="C418" s="2"/>
       <c r="E418" s="1"/>
     </row>
-    <row r="419" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A419" s="1"/>
       <c r="C419" s="2"/>
       <c r="E419" s="1"/>
     </row>
-    <row r="420" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A420" s="1"/>
       <c r="C420" s="2"/>
       <c r="E420" s="1"/>
     </row>
-    <row r="421" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A421" s="1"/>
       <c r="C421" s="2"/>
       <c r="E421" s="1"/>
     </row>
-    <row r="422" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A422" s="1"/>
       <c r="C422" s="2"/>
       <c r="E422" s="1"/>
     </row>
-    <row r="423" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A423" s="1"/>
       <c r="C423" s="2"/>
       <c r="E423" s="1"/>
     </row>
-    <row r="424" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A424" s="1"/>
       <c r="C424" s="2"/>
       <c r="E424" s="1"/>
     </row>
-    <row r="425" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A425" s="1"/>
       <c r="C425" s="2"/>
       <c r="E425" s="1"/>
     </row>
-    <row r="426" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A426" s="1"/>
       <c r="C426" s="2"/>
       <c r="E426" s="1"/>
     </row>
-    <row r="427" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A427" s="1"/>
       <c r="C427" s="2"/>
       <c r="E427" s="1"/>
     </row>
-    <row r="428" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A428" s="1"/>
       <c r="C428" s="2"/>
       <c r="E428" s="1"/>
     </row>
-    <row r="429" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A429" s="1"/>
       <c r="C429" s="2"/>
       <c r="E429" s="1"/>
     </row>
-    <row r="430" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A430" s="1"/>
       <c r="C430" s="3"/>
       <c r="E430" s="1"/>
     </row>
-    <row r="431" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A431" s="1"/>
       <c r="C431" s="3"/>
       <c r="E431" s="1"/>
     </row>
-    <row r="432" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A432" s="1"/>
       <c r="C432" s="3"/>
       <c r="E432" s="1"/>
     </row>
-    <row r="433" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A433" s="1"/>
       <c r="C433" s="2"/>
       <c r="E433" s="1"/>
     </row>
-    <row r="434" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A434" s="1"/>
       <c r="C434" s="2"/>
       <c r="E434" s="1"/>
     </row>
-    <row r="435" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A435" s="1"/>
       <c r="C435" s="2"/>
       <c r="E435" s="1"/>
     </row>
-    <row r="436" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A436" s="1"/>
       <c r="C436" s="3"/>
       <c r="E436" s="1"/>
     </row>
-    <row r="437" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A437" s="1"/>
       <c r="C437" s="3"/>
       <c r="E437" s="1"/>
     </row>
-    <row r="438" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A438" s="1"/>
       <c r="C438" s="3"/>
       <c r="E438" s="1"/>
     </row>
-    <row r="439" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A439" s="1"/>
       <c r="C439" s="3"/>
       <c r="E439" s="1"/>
     </row>
-    <row r="440" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A440" s="1"/>
       <c r="C440" s="3"/>
       <c r="E440" s="1"/>
     </row>
-    <row r="441" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A441" s="1"/>
       <c r="C441" s="3"/>
       <c r="E441" s="1"/>
     </row>
-    <row r="442" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A442" s="1"/>
       <c r="C442" s="2"/>
       <c r="E442" s="1"/>
     </row>
-    <row r="443" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A443" s="1"/>
       <c r="C443" s="2"/>
       <c r="E443" s="1"/>
     </row>
-    <row r="444" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A444" s="1"/>
       <c r="C444" s="2"/>
       <c r="E444" s="1"/>
     </row>
-    <row r="445" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A445" s="1"/>
       <c r="C445" s="2"/>
       <c r="E445" s="1"/>
     </row>
-    <row r="446" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A446" s="1"/>
       <c r="C446" s="2"/>
       <c r="E446" s="1"/>
     </row>
-    <row r="447" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A447" s="1"/>
       <c r="C447" s="2"/>
       <c r="E447" s="1"/>
     </row>
-    <row r="448" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A448" s="1"/>
       <c r="C448" s="2"/>
       <c r="E448" s="1"/>
     </row>
-    <row r="449" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A449" s="1"/>
       <c r="C449" s="2"/>
       <c r="E449" s="1"/>
     </row>
-    <row r="450" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A450" s="1"/>
       <c r="C450" s="2"/>
       <c r="E450" s="1"/>
     </row>
-    <row r="451" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A451" s="1"/>
       <c r="C451" s="2"/>
       <c r="E451" s="1"/>
     </row>
-    <row r="452" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A452" s="1"/>
       <c r="C452" s="2"/>
       <c r="E452" s="1"/>
     </row>
-    <row r="453" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A453" s="1"/>
       <c r="C453" s="2"/>
       <c r="E453" s="1"/>
     </row>
-    <row r="454" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A454" s="1"/>
       <c r="C454" s="2"/>
       <c r="E454" s="1"/>
     </row>
-    <row r="455" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A455" s="1"/>
       <c r="C455" s="2"/>
       <c r="E455" s="1"/>
     </row>
-    <row r="456" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A456" s="1"/>
       <c r="C456" s="2"/>
       <c r="E456" s="1"/>
     </row>
-    <row r="457" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A457" s="1"/>
       <c r="C457" s="2"/>
       <c r="E457" s="1"/>
     </row>
-    <row r="458" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A458" s="1"/>
       <c r="C458" s="2"/>
       <c r="E458" s="1"/>
     </row>
-    <row r="459" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A459" s="1"/>
       <c r="C459" s="2"/>
       <c r="E459" s="1"/>
     </row>
-    <row r="460" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A460" s="1"/>
       <c r="C460" s="3"/>
       <c r="E460" s="1"/>
     </row>
-    <row r="461" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A461" s="1"/>
       <c r="C461" s="3"/>
       <c r="E461" s="1"/>
     </row>
-    <row r="462" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A462" s="1"/>
       <c r="C462" s="3"/>
       <c r="E462" s="1"/>
     </row>
-    <row r="463" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A463" s="1"/>
       <c r="C463" s="2"/>
       <c r="E463" s="1"/>
     </row>
-    <row r="464" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A464" s="1"/>
       <c r="C464" s="2"/>
       <c r="E464" s="1"/>
     </row>
-    <row r="465" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A465" s="1"/>
       <c r="C465" s="2"/>
       <c r="E465" s="1"/>
     </row>
-    <row r="466" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A466" s="1"/>
       <c r="C466" s="2"/>
       <c r="E466" s="1"/>
     </row>
-    <row r="467" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A467" s="1"/>
       <c r="C467" s="2"/>
       <c r="E467" s="1"/>
     </row>
-    <row r="468" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A468" s="1"/>
       <c r="C468" s="2"/>
       <c r="E468" s="1"/>
     </row>
-    <row r="469" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A469" s="1"/>
       <c r="C469" s="2"/>
       <c r="E469" s="1"/>
     </row>
-    <row r="470" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A470" s="1"/>
       <c r="C470" s="2"/>
       <c r="E470" s="1"/>
     </row>
-    <row r="471" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A471" s="1"/>
       <c r="C471" s="2"/>
       <c r="E471" s="1"/>
     </row>
-    <row r="472" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A472" s="1"/>
       <c r="C472" s="2"/>
       <c r="E472" s="1"/>
     </row>
-    <row r="473" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A473" s="1"/>
       <c r="C473" s="2"/>
       <c r="E473" s="1"/>
     </row>
-    <row r="474" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A474" s="1"/>
       <c r="C474" s="2"/>
       <c r="E474" s="1"/>
     </row>
-    <row r="475" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A475" s="1"/>
       <c r="C475" s="2"/>
       <c r="E475" s="1"/>
     </row>
-    <row r="476" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A476" s="1"/>
       <c r="C476" s="2"/>
       <c r="E476" s="1"/>
     </row>
-    <row r="477" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A477" s="1"/>
       <c r="C477" s="2"/>
       <c r="E477" s="1"/>
     </row>
-    <row r="478" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A478" s="1"/>
       <c r="C478" s="2"/>
       <c r="E478" s="1"/>
     </row>
-    <row r="479" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A479" s="1"/>
       <c r="C479" s="2"/>
       <c r="E479" s="1"/>
     </row>
-    <row r="480" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A480" s="1"/>
       <c r="C480" s="2"/>
       <c r="E480" s="1"/>
     </row>
-    <row r="481" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A481" s="1"/>
       <c r="C481" s="2"/>
       <c r="E481" s="1"/>
     </row>
-    <row r="482" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A482" s="1"/>
       <c r="C482" s="2"/>
       <c r="E482" s="1"/>
     </row>
-    <row r="483" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A483" s="1"/>
       <c r="C483" s="2"/>
       <c r="E483" s="1"/>
     </row>
-    <row r="484" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A484" s="1"/>
       <c r="C484" s="2"/>
       <c r="E484" s="1"/>
     </row>
-    <row r="485" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A485" s="1"/>
       <c r="C485" s="2"/>
       <c r="E485" s="1"/>
     </row>
-    <row r="486" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A486" s="1"/>
       <c r="C486" s="2"/>
       <c r="E486" s="1"/>
     </row>
-    <row r="487" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A487" s="1"/>
       <c r="C487" s="2"/>
       <c r="E487" s="1"/>
     </row>
-    <row r="488" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A488" s="1"/>
       <c r="C488" s="2"/>
       <c r="E488" s="1"/>
     </row>
-    <row r="489" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A489" s="1"/>
       <c r="C489" s="2"/>
       <c r="E489" s="1"/>
     </row>
-    <row r="490" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A490" s="1"/>
       <c r="C490" s="2"/>
       <c r="E490" s="1"/>
     </row>
-    <row r="491" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A491" s="1"/>
       <c r="C491" s="2"/>
       <c r="E491" s="1"/>
     </row>
-    <row r="492" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A492" s="1"/>
       <c r="C492" s="2"/>
       <c r="E492" s="1"/>
     </row>
-    <row r="493" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A493" s="1"/>
       <c r="C493" s="2"/>
       <c r="E493" s="1"/>
     </row>
-    <row r="494" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A494" s="1"/>
       <c r="C494" s="2"/>
       <c r="E494" s="1"/>
     </row>
-    <row r="495" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A495" s="1"/>
       <c r="C495" s="2"/>
       <c r="E495" s="1"/>
     </row>
-    <row r="496" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A496" s="1"/>
       <c r="C496" s="2"/>
       <c r="E496" s="1"/>
     </row>
-    <row r="497" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A497" s="1"/>
       <c r="C497" s="2"/>
       <c r="E497" s="1"/>
     </row>
-    <row r="498" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A498" s="1"/>
       <c r="C498" s="2"/>
       <c r="E498" s="1"/>
     </row>
-    <row r="499" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A499" s="1"/>
       <c r="C499" s="2"/>
       <c r="E499" s="1"/>
     </row>
-    <row r="500" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A500" s="1"/>
       <c r="C500" s="2"/>
       <c r="E500" s="1"/>
     </row>
-    <row r="501" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A501" s="1"/>
       <c r="C501" s="2"/>
       <c r="E501" s="1"/>
     </row>
-    <row r="502" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A502" s="1"/>
       <c r="C502" s="3"/>
       <c r="E502" s="1"/>
     </row>
-    <row r="503" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A503" s="1"/>
       <c r="C503" s="3"/>
       <c r="E503" s="1"/>
     </row>
-    <row r="504" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A504" s="1"/>
       <c r="C504" s="3"/>
       <c r="E504" s="1"/>
     </row>
-    <row r="505" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A505" s="1"/>
       <c r="C505" s="2"/>
       <c r="E505" s="1"/>
     </row>
-    <row r="506" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A506" s="1"/>
       <c r="C506" s="2"/>
       <c r="E506" s="1"/>
     </row>
-    <row r="507" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A507" s="1"/>
       <c r="C507" s="2"/>
       <c r="E507" s="1"/>
     </row>
-    <row r="508" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A508" s="1"/>
       <c r="C508" s="2"/>
       <c r="E508" s="1"/>
     </row>
-    <row r="509" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A509" s="1"/>
       <c r="C509" s="2"/>
       <c r="E509" s="1"/>
     </row>
-    <row r="510" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A510" s="1"/>
       <c r="C510" s="2"/>
       <c r="E510" s="1"/>
     </row>
-    <row r="511" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A511" s="1"/>
       <c r="C511" s="2"/>
       <c r="E511" s="1"/>
     </row>
-    <row r="512" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A512" s="1"/>
       <c r="C512" s="2"/>
       <c r="E512" s="1"/>
     </row>
-    <row r="513" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A513" s="1"/>
       <c r="C513" s="2"/>
       <c r="E513" s="1"/>
     </row>
-    <row r="514" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A514" s="1"/>
       <c r="C514" s="2"/>
       <c r="E514" s="1"/>
     </row>
-    <row r="515" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A515" s="1"/>
       <c r="C515" s="2"/>
       <c r="E515" s="1"/>
     </row>
-    <row r="516" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A516" s="1"/>
       <c r="C516" s="2"/>
       <c r="E516" s="1"/>
     </row>
-    <row r="517" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A517" s="1"/>
       <c r="C517" s="2"/>
       <c r="E517" s="1"/>
     </row>
-    <row r="518" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A518" s="1"/>
       <c r="C518" s="2"/>
       <c r="E518" s="1"/>
     </row>
-    <row r="519" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A519" s="1"/>
       <c r="C519" s="2"/>
       <c r="E519" s="1"/>
     </row>
-    <row r="520" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A520" s="1"/>
       <c r="C520" s="2"/>
       <c r="E520" s="1"/>
     </row>
-    <row r="521" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A521" s="1"/>
       <c r="C521" s="2"/>
       <c r="E521" s="1"/>
     </row>
-    <row r="522" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A522" s="1"/>
       <c r="C522" s="2"/>
       <c r="E522" s="1"/>
     </row>
-    <row r="523" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A523" s="1"/>
       <c r="C523" s="2"/>
       <c r="E523" s="1"/>
     </row>
-    <row r="524" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A524" s="1"/>
       <c r="C524" s="2"/>
       <c r="E524" s="1"/>
     </row>
-    <row r="525" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A525" s="1"/>
       <c r="C525" s="2"/>
       <c r="E525" s="1"/>
     </row>
-    <row r="526" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A526" s="1"/>
       <c r="C526" s="2"/>
       <c r="E526" s="1"/>
     </row>
-    <row r="527" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A527" s="1"/>
       <c r="C527" s="2"/>
       <c r="E527" s="1"/>
     </row>
-    <row r="528" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A528" s="1"/>
       <c r="C528" s="2"/>
       <c r="E528" s="1"/>
     </row>
-    <row r="529" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A529" s="1"/>
       <c r="C529" s="2"/>
       <c r="E529" s="1"/>
     </row>
-    <row r="530" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A530" s="1"/>
       <c r="C530" s="2"/>
       <c r="E530" s="1"/>
     </row>
-    <row r="531" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A531" s="1"/>
       <c r="C531" s="2"/>
       <c r="E531" s="1"/>
     </row>
-    <row r="532" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A532" s="1"/>
       <c r="C532" s="3"/>
       <c r="E532" s="1"/>
     </row>
-    <row r="533" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A533" s="1"/>
       <c r="C533" s="3"/>
       <c r="E533" s="1"/>
     </row>
-    <row r="534" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A534" s="1"/>
       <c r="C534" s="3"/>
       <c r="E534" s="1"/>
     </row>
-    <row r="535" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A535" s="1"/>
       <c r="C535" s="2"/>
       <c r="E535" s="1"/>
     </row>
-    <row r="536" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A536" s="1"/>
       <c r="C536" s="2"/>
       <c r="E536" s="1"/>
     </row>
-    <row r="537" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A537" s="1"/>
       <c r="C537" s="2"/>
       <c r="E537" s="1"/>
     </row>
-    <row r="538" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A538" s="1"/>
       <c r="C538" s="3"/>
       <c r="E538" s="1"/>
     </row>
-    <row r="539" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A539" s="1"/>
       <c r="C539" s="3"/>
       <c r="E539" s="1"/>
     </row>
-    <row r="540" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A540" s="1"/>
       <c r="C540" s="3"/>
       <c r="E540" s="1"/>
     </row>
-    <row r="541" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A541" s="1"/>
       <c r="C541" s="2"/>
       <c r="E541" s="1"/>
     </row>
-    <row r="542" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A542" s="1"/>
       <c r="C542" s="2"/>
       <c r="E542" s="1"/>
     </row>
-    <row r="543" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A543" s="1"/>
       <c r="C543" s="2"/>
       <c r="E543" s="1"/>
     </row>
-    <row r="544" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A544" s="1"/>
       <c r="C544" s="2"/>
       <c r="E544" s="1"/>
     </row>
-    <row r="545" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A545" s="1"/>
       <c r="C545" s="2"/>
       <c r="E545" s="1"/>
     </row>
-    <row r="546" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A546" s="1"/>
       <c r="C546" s="2"/>
       <c r="E546" s="1"/>
     </row>
-    <row r="547" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A547" s="1"/>
       <c r="C547" s="2"/>
       <c r="E547" s="1"/>
     </row>
-    <row r="548" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A548" s="1"/>
       <c r="C548" s="2"/>
       <c r="E548" s="1"/>
     </row>
-    <row r="549" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A549" s="1"/>
       <c r="C549" s="2"/>
       <c r="E549" s="1"/>
     </row>
-    <row r="550" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A550" s="1"/>
       <c r="C550" s="2"/>
       <c r="E550" s="1"/>
     </row>
-    <row r="551" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A551" s="1"/>
       <c r="C551" s="2"/>
       <c r="E551" s="1"/>
     </row>
-    <row r="552" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A552" s="1"/>
       <c r="C552" s="2"/>
       <c r="E552" s="1"/>
     </row>
-    <row r="553" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="553" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A553" s="1"/>
       <c r="C553" s="2"/>
       <c r="E553" s="1"/>
     </row>
-    <row r="554" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A554" s="1"/>
       <c r="C554" s="2"/>
       <c r="E554" s="1"/>
     </row>
-    <row r="555" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A555" s="1"/>
       <c r="C555" s="2"/>
       <c r="E555" s="1"/>
     </row>
-    <row r="556" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A556" s="1"/>
       <c r="C556" s="2"/>
       <c r="E556" s="1"/>
     </row>
-    <row r="557" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="557" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A557" s="1"/>
       <c r="C557" s="2"/>
       <c r="E557" s="1"/>
     </row>
-    <row r="558" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A558" s="1"/>
       <c r="C558" s="2"/>
       <c r="E558" s="1"/>
     </row>
-    <row r="559" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A559" s="1"/>
       <c r="C559" s="2"/>
       <c r="E559" s="1"/>
     </row>
-    <row r="560" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A560" s="1"/>
       <c r="C560" s="2"/>
       <c r="E560" s="1"/>
     </row>
-    <row r="561" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A561" s="1"/>
       <c r="C561" s="2"/>
       <c r="E561" s="1"/>
     </row>
-    <row r="562" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="562" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A562" s="1"/>
       <c r="C562" s="2"/>
       <c r="E562" s="1"/>
     </row>
-    <row r="563" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="563" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A563" s="1"/>
       <c r="C563" s="2"/>
       <c r="E563" s="1"/>
     </row>
-    <row r="564" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="564" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A564" s="1"/>
       <c r="C564" s="2"/>
       <c r="E564" s="1"/>
     </row>
-    <row r="565" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A565" s="1"/>
       <c r="C565" s="3"/>
       <c r="E565" s="1"/>
     </row>
-    <row r="566" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="566" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A566" s="1"/>
       <c r="C566" s="3"/>
       <c r="E566" s="1"/>
     </row>
-    <row r="567" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A567" s="1"/>
       <c r="C567" s="3"/>
       <c r="E567" s="1"/>
     </row>
-    <row r="568" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A568" s="1"/>
       <c r="C568" s="2"/>
       <c r="E568" s="1"/>
     </row>
-    <row r="569" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="569" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A569" s="1"/>
       <c r="C569" s="2"/>
       <c r="E569" s="1"/>
     </row>
-    <row r="570" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A570" s="1"/>
       <c r="C570" s="2"/>
       <c r="E570" s="1"/>
     </row>
-    <row r="571" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="571" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A571" s="1"/>
       <c r="C571" s="2"/>
       <c r="E571" s="1"/>
     </row>
-    <row r="572" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="572" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A572" s="1"/>
       <c r="C572" s="2"/>
       <c r="E572" s="1"/>
     </row>
-    <row r="573" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="573" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A573" s="1"/>
       <c r="C573" s="2"/>
       <c r="E573" s="1"/>
     </row>
-    <row r="574" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="574" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A574" s="1"/>
       <c r="C574" s="3"/>
       <c r="E574" s="1"/>
     </row>
-    <row r="575" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="575" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A575" s="1"/>
       <c r="C575" s="3"/>
       <c r="E575" s="1"/>
     </row>
-    <row r="576" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A576" s="1"/>
       <c r="C576" s="3"/>
       <c r="E576" s="1"/>
     </row>
-    <row r="577" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="577" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A577" s="1"/>
       <c r="C577" s="2"/>
       <c r="E577" s="1"/>
     </row>
-    <row r="578" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="578" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A578" s="1"/>
       <c r="C578" s="2"/>
       <c r="E578" s="1"/>
     </row>
-    <row r="579" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="579" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A579" s="1"/>
       <c r="C579" s="2"/>
       <c r="E579" s="1"/>
     </row>
-    <row r="580" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="580" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A580" s="1"/>
       <c r="C580" s="2"/>
       <c r="E580" s="1"/>
     </row>
-    <row r="581" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="581" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A581" s="1"/>
       <c r="C581" s="2"/>
       <c r="E581" s="1"/>
     </row>
-    <row r="582" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="582" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A582" s="1"/>
       <c r="C582" s="2"/>
       <c r="E582" s="1"/>
     </row>
-    <row r="583" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="583" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A583" s="1"/>
       <c r="C583" s="2"/>
       <c r="E583" s="1"/>
     </row>
-    <row r="584" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="584" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A584" s="1"/>
       <c r="C584" s="2"/>
       <c r="E584" s="1"/>
     </row>
-    <row r="585" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="585" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A585" s="1"/>
       <c r="C585" s="2"/>
       <c r="E585" s="1"/>
     </row>
-    <row r="586" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A586" s="1"/>
       <c r="C586" s="3"/>
       <c r="E586" s="1"/>
     </row>
-    <row r="587" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="587" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A587" s="1"/>
       <c r="C587" s="3"/>
       <c r="E587" s="1"/>
     </row>
-    <row r="588" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="588" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A588" s="1"/>
       <c r="C588" s="3"/>
       <c r="E588" s="1"/>
     </row>
-    <row r="589" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="589" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A589" s="1"/>
       <c r="C589" s="3"/>
       <c r="E589" s="1"/>
     </row>
-    <row r="590" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="590" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A590" s="1"/>
       <c r="C590" s="3"/>
       <c r="E590" s="1"/>
     </row>
-    <row r="591" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="591" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A591" s="1"/>
       <c r="C591" s="3"/>
       <c r="E591" s="1"/>
     </row>
-    <row r="592" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="592" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A592" s="1"/>
       <c r="C592" s="2"/>
       <c r="E592" s="1"/>
     </row>
-    <row r="593" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A593" s="1"/>
       <c r="C593" s="2"/>
       <c r="E593" s="1"/>
     </row>
-    <row r="594" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A594" s="1"/>
       <c r="C594" s="2"/>
       <c r="E594" s="1"/>
     </row>
-    <row r="595" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="595" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A595" s="1"/>
       <c r="C595" s="2"/>
       <c r="E595" s="1"/>
     </row>
-    <row r="596" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A596" s="1"/>
       <c r="C596" s="2"/>
       <c r="E596" s="1"/>
     </row>
-    <row r="597" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A597" s="1"/>
       <c r="C597" s="2"/>
       <c r="E597" s="1"/>
     </row>
-    <row r="598" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="598" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A598" s="1"/>
       <c r="C598" s="2"/>
       <c r="E598" s="1"/>
     </row>
-    <row r="599" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="599" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A599" s="1"/>
       <c r="C599" s="2"/>
       <c r="E599" s="1"/>
     </row>
-    <row r="600" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A600" s="1"/>
       <c r="C600" s="2"/>
       <c r="E600" s="1"/>
     </row>
-    <row r="601" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="601" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A601" s="1"/>
       <c r="C601" s="2"/>
       <c r="E601" s="1"/>
     </row>
-    <row r="602" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="602" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A602" s="1"/>
       <c r="C602" s="2"/>
       <c r="E602" s="1"/>
     </row>
-    <row r="603" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="603" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A603" s="1"/>
       <c r="C603" s="2"/>
       <c r="E603" s="1"/>
     </row>
-    <row r="604" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A604" s="1"/>
       <c r="C604" s="3"/>
       <c r="E604" s="1"/>
     </row>
-    <row r="605" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="605" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A605" s="1"/>
       <c r="C605" s="3"/>
       <c r="E605" s="1"/>
     </row>
-    <row r="606" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A606" s="1"/>
       <c r="C606" s="3"/>
       <c r="E606" s="1"/>
     </row>
-    <row r="607" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A607" s="1"/>
       <c r="C607" s="2"/>
       <c r="E607" s="1"/>
     </row>
-    <row r="608" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A608" s="1"/>
       <c r="C608" s="2"/>
       <c r="E608" s="1"/>
     </row>
-    <row r="609" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A609" s="1"/>
       <c r="C609" s="2"/>
       <c r="E609" s="1"/>
     </row>
-    <row r="610" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A610" s="1"/>
       <c r="C610" s="2"/>
       <c r="E610" s="1"/>
     </row>
-    <row r="611" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="611" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A611" s="1"/>
       <c r="C611" s="2"/>
       <c r="E611" s="1"/>
     </row>
-    <row r="612" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="612" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A612" s="1"/>
       <c r="C612" s="2"/>
       <c r="E612" s="1"/>
     </row>
-    <row r="613" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="613" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A613" s="1"/>
       <c r="C613" s="2"/>
       <c r="E613" s="1"/>
     </row>
-    <row r="614" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="614" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A614" s="1"/>
       <c r="C614" s="2"/>
       <c r="E614" s="1"/>
     </row>
-    <row r="615" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A615" s="1"/>
       <c r="C615" s="2"/>
       <c r="E615" s="1"/>
     </row>
-    <row r="616" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="616" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A616" s="1"/>
       <c r="C616" s="2"/>
       <c r="E616" s="1"/>
     </row>
-    <row r="617" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="617" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A617" s="1"/>
       <c r="C617" s="2"/>
       <c r="E617" s="1"/>
     </row>
-    <row r="618" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A618" s="1"/>
       <c r="C618" s="2"/>
       <c r="E618" s="1"/>
     </row>
-    <row r="619" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="619" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A619" s="1"/>
       <c r="C619" s="2"/>
       <c r="E619" s="1"/>
     </row>
-    <row r="620" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="620" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A620" s="1"/>
       <c r="C620" s="2"/>
       <c r="E620" s="1"/>
     </row>
-    <row r="621" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="621" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A621" s="1"/>
       <c r="C621" s="2"/>
       <c r="E621" s="1"/>
     </row>
-    <row r="622" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="622" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A622" s="1"/>
       <c r="C622" s="2"/>
       <c r="E622" s="1"/>
     </row>
-    <row r="623" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="623" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A623" s="1"/>
       <c r="C623" s="2"/>
       <c r="E623" s="1"/>
     </row>
-    <row r="624" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="624" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A624" s="1"/>
       <c r="C624" s="2"/>
       <c r="E624" s="1"/>
     </row>
-    <row r="625" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="625" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A625" s="1"/>
       <c r="C625" s="3"/>
       <c r="E625" s="1"/>
     </row>
-    <row r="626" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="626" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A626" s="1"/>
       <c r="C626" s="3"/>
       <c r="E626" s="1"/>
     </row>
-    <row r="627" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="627" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A627" s="1"/>
       <c r="C627" s="3"/>
       <c r="E627" s="1"/>
     </row>
-    <row r="628" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="628" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A628" s="1"/>
       <c r="C628" s="2"/>
       <c r="E628" s="1"/>
     </row>
-    <row r="629" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="629" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A629" s="1"/>
       <c r="C629" s="2"/>
       <c r="E629" s="1"/>
     </row>
-    <row r="630" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="630" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A630" s="1"/>
       <c r="C630" s="2"/>
       <c r="E630" s="1"/>
     </row>
-    <row r="631" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="631" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A631" s="1"/>
       <c r="C631" s="2"/>
       <c r="E631" s="1"/>
     </row>
-    <row r="632" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="632" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A632" s="1"/>
       <c r="C632" s="2"/>
       <c r="E632" s="1"/>
     </row>
-    <row r="633" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="633" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A633" s="1"/>
       <c r="C633" s="2"/>
       <c r="E633" s="1"/>
     </row>
-    <row r="634" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="634" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A634" s="1"/>
       <c r="C634" s="2"/>
       <c r="E634" s="1"/>
     </row>
-    <row r="635" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="635" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A635" s="1"/>
       <c r="C635" s="2"/>
       <c r="E635" s="1"/>
     </row>
-    <row r="636" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="636" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A636" s="1"/>
       <c r="C636" s="2"/>
       <c r="E636" s="1"/>
     </row>
-    <row r="637" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="637" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A637" s="1"/>
       <c r="C637" s="2"/>
       <c r="E637" s="1"/>
     </row>
-    <row r="638" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="638" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A638" s="1"/>
       <c r="C638" s="2"/>
       <c r="E638" s="1"/>
     </row>
-    <row r="639" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="639" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A639" s="1"/>
       <c r="C639" s="2"/>
       <c r="E639" s="1"/>
     </row>
-    <row r="640" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="640" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A640" s="1"/>
       <c r="C640" s="2"/>
       <c r="E640" s="1"/>
     </row>
-    <row r="641" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="641" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A641" s="1"/>
       <c r="C641" s="2"/>
       <c r="E641" s="1"/>
     </row>
-    <row r="642" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="642" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A642" s="1"/>
       <c r="C642" s="2"/>
       <c r="E642" s="1"/>
     </row>
-    <row r="643" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="643" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A643" s="1"/>
       <c r="C643" s="2"/>
       <c r="E643" s="1"/>
     </row>
-    <row r="644" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="644" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A644" s="1"/>
       <c r="C644" s="2"/>
       <c r="E644" s="1"/>
     </row>
-    <row r="645" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="645" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A645" s="1"/>
       <c r="C645" s="2"/>
       <c r="E645" s="1"/>
     </row>
-    <row r="646" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="646" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A646" s="1"/>
       <c r="C646" s="2"/>
       <c r="E646" s="1"/>
     </row>
-    <row r="647" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="647" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A647" s="1"/>
       <c r="C647" s="2"/>
       <c r="E647" s="1"/>
     </row>
-    <row r="648" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="648" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A648" s="1"/>
       <c r="C648" s="2"/>
       <c r="E648" s="1"/>
     </row>
-    <row r="649" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="649" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A649" s="1"/>
       <c r="C649" s="2"/>
       <c r="E649" s="1"/>
     </row>
-    <row r="650" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="650" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A650" s="1"/>
       <c r="C650" s="2"/>
       <c r="E650" s="1"/>
     </row>
-    <row r="651" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="651" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A651" s="1"/>
       <c r="C651" s="2"/>
       <c r="E651" s="1"/>
     </row>
-    <row r="652" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="652" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A652" s="1"/>
       <c r="C652" s="2"/>
       <c r="E652" s="1"/>
     </row>
-    <row r="653" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="653" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A653" s="1"/>
       <c r="C653" s="2"/>
       <c r="E653" s="1"/>
     </row>
-    <row r="654" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="654" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A654" s="1"/>
       <c r="C654" s="2"/>
       <c r="E654" s="1"/>
     </row>
-    <row r="655" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="655" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A655" s="1"/>
       <c r="C655" s="2"/>
       <c r="E655" s="1"/>
     </row>
-    <row r="656" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="656" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A656" s="1"/>
       <c r="C656" s="2"/>
       <c r="E656" s="1"/>
     </row>
-    <row r="657" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="657" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A657" s="1"/>
       <c r="C657" s="2"/>
       <c r="E657" s="1"/>
     </row>
-    <row r="658" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="658" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A658" s="1"/>
       <c r="C658" s="2"/>
       <c r="E658" s="1"/>
     </row>
-    <row r="659" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="659" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A659" s="1"/>
       <c r="C659" s="2"/>
       <c r="E659" s="1"/>
     </row>
-    <row r="660" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="660" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A660" s="1"/>
       <c r="C660" s="2"/>
       <c r="E660" s="1"/>
     </row>
-    <row r="661" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="661" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A661" s="1"/>
       <c r="C661" s="2"/>
       <c r="E661" s="1"/>
     </row>
-    <row r="662" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="662" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A662" s="1"/>
       <c r="C662" s="2"/>
       <c r="E662" s="1"/>
     </row>
-    <row r="663" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="663" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A663" s="1"/>
       <c r="C663" s="2"/>
       <c r="E663" s="1"/>
     </row>
-    <row r="664" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="664" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A664" s="1"/>
       <c r="C664" s="3"/>
       <c r="E664" s="1"/>
     </row>
-    <row r="665" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="665" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A665" s="1"/>
       <c r="C665" s="3"/>
       <c r="E665" s="1"/>
     </row>
-    <row r="666" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="666" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A666" s="1"/>
       <c r="C666" s="3"/>
       <c r="E666" s="1"/>
     </row>
-    <row r="667" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="667" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A667" s="1"/>
       <c r="C667" s="2"/>
       <c r="E667" s="1"/>
     </row>
-    <row r="668" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A668" s="1"/>
       <c r="C668" s="2"/>
       <c r="E668" s="1"/>
     </row>
-    <row r="669" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="669" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A669" s="1"/>
       <c r="C669" s="2"/>
       <c r="E669" s="1"/>
     </row>
-    <row r="670" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="670" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A670" s="1"/>
       <c r="C670" s="2"/>
       <c r="E670" s="1"/>
     </row>
-    <row r="671" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="671" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A671" s="1"/>
       <c r="C671" s="2"/>
       <c r="E671" s="1"/>
     </row>
-    <row r="672" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="672" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A672" s="1"/>
       <c r="C672" s="2"/>
       <c r="E672" s="1"/>
     </row>
-    <row r="673" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="673" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A673" s="1"/>
       <c r="C673" s="2"/>
       <c r="E673" s="1"/>
     </row>
-    <row r="674" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="674" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A674" s="1"/>
       <c r="C674" s="2"/>
       <c r="E674" s="1"/>
     </row>
-    <row r="675" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="675" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A675" s="1"/>
       <c r="C675" s="2"/>
       <c r="E675" s="1"/>
     </row>
-    <row r="676" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="676" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A676" s="1"/>
       <c r="C676" s="2"/>
       <c r="E676" s="1"/>
     </row>
-    <row r="677" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="677" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A677" s="1"/>
       <c r="C677" s="2"/>
       <c r="E677" s="1"/>
     </row>
-    <row r="678" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="678" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A678" s="1"/>
       <c r="C678" s="2"/>
       <c r="E678" s="1"/>
     </row>
-    <row r="679" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="679" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A679" s="1"/>
       <c r="C679" s="2"/>
       <c r="E679" s="1"/>
     </row>
-    <row r="680" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="680" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A680" s="1"/>
       <c r="C680" s="2"/>
       <c r="E680" s="1"/>
     </row>
-    <row r="681" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="681" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A681" s="1"/>
       <c r="C681" s="2"/>
       <c r="E681" s="1"/>
     </row>
-    <row r="682" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="682" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A682" s="1"/>
       <c r="C682" s="2"/>
       <c r="E682" s="1"/>
     </row>
-    <row r="683" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="683" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A683" s="1"/>
       <c r="C683" s="2"/>
       <c r="E683" s="1"/>
     </row>
-    <row r="684" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="684" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A684" s="1"/>
       <c r="C684" s="2"/>
       <c r="E684" s="1"/>
     </row>
-    <row r="685" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="685" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A685" s="1"/>
       <c r="C685" s="2"/>
       <c r="E685" s="1"/>
     </row>
-    <row r="686" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="686" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A686" s="1"/>
       <c r="C686" s="2"/>
       <c r="E686" s="1"/>
     </row>
-    <row r="687" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="687" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A687" s="1"/>
       <c r="C687" s="2"/>
       <c r="E687" s="1"/>
     </row>
-    <row r="688" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="688" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A688" s="1"/>
       <c r="C688" s="2"/>
       <c r="E688" s="1"/>
     </row>
-    <row r="689" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="689" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A689" s="1"/>
       <c r="C689" s="2"/>
       <c r="E689" s="1"/>
     </row>
-    <row r="690" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="690" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A690" s="1"/>
       <c r="C690" s="2"/>
       <c r="E690" s="1"/>
     </row>
-    <row r="691" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="691" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A691" s="1"/>
       <c r="C691" s="2"/>
       <c r="E691" s="1"/>
     </row>
-    <row r="692" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="692" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A692" s="1"/>
       <c r="C692" s="2"/>
       <c r="E692" s="1"/>
     </row>
-    <row r="693" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="693" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A693" s="1"/>
       <c r="C693" s="2"/>
       <c r="E693" s="1"/>
     </row>
-    <row r="694" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="694" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A694" s="1"/>
       <c r="C694" s="2"/>
       <c r="E694" s="1"/>
     </row>
-    <row r="695" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="695" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A695" s="1"/>
       <c r="C695" s="2"/>
       <c r="E695" s="1"/>
     </row>
-    <row r="696" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="696" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A696" s="1"/>
       <c r="C696" s="2"/>
       <c r="E696" s="1"/>
     </row>
-    <row r="697" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="697" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A697" s="1"/>
       <c r="C697" s="2"/>
       <c r="E697" s="1"/>
     </row>
-    <row r="698" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="698" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A698" s="1"/>
       <c r="C698" s="2"/>
       <c r="E698" s="1"/>
     </row>
-    <row r="699" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="699" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A699" s="1"/>
       <c r="C699" s="2"/>
       <c r="E699" s="1"/>
     </row>
-    <row r="700" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="700" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A700" s="1"/>
       <c r="C700" s="2"/>
       <c r="E700" s="1"/>
     </row>
-    <row r="701" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="701" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A701" s="1"/>
       <c r="C701" s="2"/>
       <c r="E701" s="1"/>
     </row>
-    <row r="702" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="702" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A702" s="1"/>
       <c r="C702" s="2"/>
       <c r="E702" s="1"/>
     </row>
-    <row r="703" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="703" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A703" s="1"/>
       <c r="C703" s="2"/>
       <c r="E703" s="1"/>
     </row>
-    <row r="704" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="704" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A704" s="1"/>
       <c r="C704" s="2"/>
       <c r="E704" s="1"/>
     </row>
-    <row r="705" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="705" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A705" s="1"/>
       <c r="C705" s="2"/>
       <c r="E705" s="1"/>
     </row>
-    <row r="706" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="706" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A706" s="1"/>
       <c r="C706" s="3"/>
       <c r="E706" s="1"/>
     </row>
-    <row r="707" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="707" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A707" s="1"/>
       <c r="C707" s="3"/>
       <c r="E707" s="1"/>
     </row>
-    <row r="708" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="708" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A708" s="1"/>
       <c r="C708" s="3"/>
       <c r="E708" s="1"/>
     </row>
-    <row r="709" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="709" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A709" s="1"/>
       <c r="C709" s="2"/>
       <c r="E709" s="1"/>
     </row>
-    <row r="710" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="710" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A710" s="1"/>
       <c r="C710" s="2"/>
       <c r="E710" s="1"/>
     </row>
-    <row r="711" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="711" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A711" s="1"/>
       <c r="C711" s="2"/>
       <c r="E711" s="1"/>
     </row>
-    <row r="712" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="712" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A712" s="1"/>
       <c r="C712" s="2"/>
       <c r="E712" s="1"/>
     </row>
-    <row r="713" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="713" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A713" s="1"/>
       <c r="C713" s="2"/>
       <c r="E713" s="1"/>
     </row>
-    <row r="714" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="714" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A714" s="1"/>
       <c r="C714" s="2"/>
       <c r="E714" s="1"/>
     </row>
-    <row r="715" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="715" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A715" s="1"/>
       <c r="C715" s="3"/>
       <c r="E715" s="1"/>
     </row>
-    <row r="716" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="716" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A716" s="1"/>
       <c r="C716" s="3"/>
       <c r="E716" s="1"/>
     </row>
-    <row r="717" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="717" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A717" s="1"/>
       <c r="C717" s="3"/>
       <c r="E717" s="1"/>
     </row>
-    <row r="718" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="718" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A718" s="1"/>
       <c r="C718" s="3"/>
       <c r="E718" s="1"/>
     </row>
-    <row r="719" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="719" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A719" s="1"/>
       <c r="C719" s="3"/>
       <c r="E719" s="1"/>
     </row>
-    <row r="720" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="720" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A720" s="1"/>
       <c r="C720" s="3"/>
       <c r="E720" s="1"/>
     </row>
-    <row r="721" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="721" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A721" s="1"/>
       <c r="C721" s="2"/>
       <c r="E721" s="1"/>
     </row>
-    <row r="722" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="722" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A722" s="1"/>
       <c r="C722" s="2"/>
       <c r="E722" s="1"/>
     </row>
-    <row r="723" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="723" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A723" s="1"/>
       <c r="C723" s="2"/>
       <c r="E723" s="1"/>
     </row>
-    <row r="724" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="724" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A724" s="1"/>
       <c r="C724" s="3"/>
       <c r="E724" s="1"/>
     </row>
-    <row r="725" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="725" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A725" s="1"/>
       <c r="C725" s="3"/>
       <c r="E725" s="1"/>
     </row>
-    <row r="726" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="726" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A726" s="1"/>
       <c r="C726" s="3"/>
       <c r="E726" s="1"/>
     </row>
-    <row r="727" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="727" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A727" s="1"/>
       <c r="C727" s="3"/>
       <c r="E727" s="1"/>
     </row>
-    <row r="728" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="728" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A728" s="1"/>
       <c r="C728" s="3"/>
       <c r="E728" s="1"/>
     </row>
-    <row r="729" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="729" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A729" s="1"/>
       <c r="C729" s="3"/>
       <c r="E729" s="1"/>
     </row>
-    <row r="730" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="730" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A730" s="1"/>
       <c r="C730" s="3"/>
       <c r="E730" s="1"/>
     </row>
-    <row r="731" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="731" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A731" s="1"/>
       <c r="C731" s="3"/>
       <c r="E731" s="1"/>
     </row>
-    <row r="732" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="732" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A732" s="1"/>
       <c r="C732" s="3"/>
       <c r="E732" s="1"/>

</xml_diff>